<commit_message>
extended vignette on ref recalibration
</commit_message>
<xml_diff>
--- a/docs/reference/report.xlsx
+++ b/docs/reference/report.xlsx
@@ -639,7 +639,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-28 10:43:25.092375</t>
+          <t>2025-04-30 17:56:50.982885</t>
         </is>
       </c>
     </row>
@@ -4396,7 +4396,7 @@
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="11.711"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="17.711"/>
     <col min="4" max="4" bestFit="1" customWidth="1" hidden="false" width="13.711"/>
     <col min="5" max="5" bestFit="1" customWidth="1" hidden="false" width="17.711"/>
     <col min="6" max="6" bestFit="1" customWidth="1" hidden="false" width="8.711"/>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>S1P d18:1</t>
+          <t>S1P d18:1 13C2D2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -5166,7 +5166,7 @@
         </is>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -5245,7 +5245,7 @@
         </is>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -5324,7 +5324,7 @@
         </is>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -5401,7 +5401,7 @@
         </is>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>S1P d18:1</t>
+          <t>S1P d18:1 13C2D2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -5478,7 +5478,7 @@
         </is>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -5557,7 +5557,7 @@
         </is>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
@@ -5636,7 +5636,7 @@
         </is>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
@@ -5715,7 +5715,7 @@
         </is>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
update docs and vignettes
</commit_message>
<xml_diff>
--- a/docs/reference/report.xlsx
+++ b/docs/reference/report.xlsx
@@ -162,7 +162,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="3" name="Table3" displayName="Table3" ref="A1:A3" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:A3"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Calibration metrics has not been calculated."/>
+    <tableColumn id="1" name="Calibration metrics have not been calculated."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -613,10 +613,10 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="18.711"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="25.711"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="27.711"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -639,7 +639,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-08 16:53:21.0599</t>
+          <t>2025-05-30 17:03:49.810467</t>
         </is>
       </c>
     </row>
@@ -712,7 +712,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="15.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
@@ -4392,7 +4392,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="14.711"/>
@@ -5775,7 +5775,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="16.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
@@ -5863,7 +5863,7 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" bestFit="1" customWidth="1" hidden="false" width="9.711"/>
     <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="15.711"/>
@@ -5929,7 +5929,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="44.711"/>
   </cols>
@@ -5976,15 +5976,15 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="45.711"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="46.711"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Calibration metrics has not been calculated.</t>
+          <t>Calibration metrics have not been calculated.</t>
         </is>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="31.711"/>
   </cols>
@@ -6070,7 +6070,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="31.711"/>
   </cols>
@@ -6117,7 +6117,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="8.711"/>
@@ -10381,7 +10381,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="8.711"/>
@@ -14645,7 +14645,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="32.711"/>
     <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="8.711"/>
@@ -18505,7 +18505,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="13.711"/>
     <col min="2" max="8" bestFit="1" customWidth="1" hidden="false" width="17.711"/>

</xml_diff>